<commit_message>
updated and finished projects
here is the updated intermediate project from when we worked on it (thank you), and also if you check the advanced folder project 1 is finished
</commit_message>
<xml_diff>
--- a/TIA copy/Excel Intermediate/Project_Int_Excel_xlsx copy.xlsx
+++ b/TIA copy/Excel Intermediate/Project_Int_Excel_xlsx copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmycreznic/Google Drive/School/Spring 2020/COS377/TIA/Excel Intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C36FF5-F92F-A346-B8D6-728BD30578D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8A19EC-177A-C24F-84E6-0FB6829A575E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="800" windowWidth="23400" windowHeight="23180" tabRatio="649" firstSheet="5" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="800" windowWidth="23400" windowHeight="23180" tabRatio="649" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="5" r:id="rId1"/>
@@ -2082,6 +2082,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2106,7 +2107,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2114,9 +2114,25 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -2136,6 +2152,12 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2230,11 +2252,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>DynamicCharts!$A$2</c:f>
+              <c:f>DynamicCharts!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Year</c:v>
+                  <c:v>Sales</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2263,7 +2285,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>DynamicCharts!$A$3:$A$16</c:f>
               <c:numCache>
@@ -2313,52 +2335,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-35E6-C944-8A4B-8B45B282B7C8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>DynamicCharts!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Sales</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>DynamicCharts!$B$3:$B$16</c:f>
@@ -2413,7 +2390,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-35E6-C944-8A4B-8B45B282B7C8}"/>
+              <c16:uniqueId val="{00000000-35E6-C944-8A4B-8B45B282B7C8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2437,6 +2414,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2501,7 +2479,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3347,11 +3325,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BC8599BC-C9AA-2446-A478-60E46AB4585C}" name="Table1" displayName="Table1" ref="A2:B16" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BC8599BC-C9AA-2446-A478-60E46AB4585C}" name="Table1" displayName="Table1" ref="A2:B17" totalsRowCount="1" headerRowDxfId="4">
   <autoFilter ref="A2:B16" xr:uid="{3BBE7E01-9687-744D-8DE9-EE94236ADC98}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0E05D6DC-B961-D64D-800D-8377849C5389}" name="Year" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{B58A5F3B-1EBD-7F4E-BCAF-EB1718D2AE27}" name="Sales" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{0E05D6DC-B961-D64D-800D-8377849C5389}" name="Year" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{B58A5F3B-1EBD-7F4E-BCAF-EB1718D2AE27}" name="Sales" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4261,8 +4239,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4315,7 +4293,7 @@
       <c r="R2" s="60"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="77">
+      <c r="A3" s="69">
         <v>2000</v>
       </c>
       <c r="B3" s="43">
@@ -4323,7 +4301,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="77">
+      <c r="A4" s="69">
         <v>2001</v>
       </c>
       <c r="B4" s="43">
@@ -4331,7 +4309,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="77">
+      <c r="A5" s="69">
         <v>2002</v>
       </c>
       <c r="B5" s="43">
@@ -4341,8 +4319,8 @@
         <v>521</v>
       </c>
       <c r="L5">
-        <f ca="1">AVERAGE(OFFSET($B$2,1,0,COUNT($B3:$B13),1))</f>
-        <v>149783.81818181818</v>
+        <f ca="1">OFFSET($B$2,1,0,COUNT($B3:$B13),1)</f>
+        <v>118348</v>
       </c>
       <c r="M5" s="68">
         <f>AVERAGE(B3:B13)</f>
@@ -4350,7 +4328,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="77">
+      <c r="A6" s="69">
         <v>2003</v>
       </c>
       <c r="B6" s="43">
@@ -4365,7 +4343,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="77">
+      <c r="A7" s="69">
         <v>2004</v>
       </c>
       <c r="B7" s="43">
@@ -4373,7 +4351,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="77">
+      <c r="A8" s="69">
         <v>2005</v>
       </c>
       <c r="B8" s="43">
@@ -4381,7 +4359,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="77">
+      <c r="A9" s="69">
         <v>2006</v>
       </c>
       <c r="B9" s="43">
@@ -4389,7 +4367,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="77">
+      <c r="A10" s="69">
         <v>2007</v>
       </c>
       <c r="B10" s="43">
@@ -4397,7 +4375,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="77">
+      <c r="A11" s="69">
         <v>2008</v>
       </c>
       <c r="B11" s="43">
@@ -4406,7 +4384,7 @@
       <c r="L11" s="66"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="77">
+      <c r="A12" s="69">
         <v>2009</v>
       </c>
       <c r="B12" s="43">
@@ -4415,7 +4393,7 @@
       <c r="L12" s="66"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="77">
+      <c r="A13" s="69">
         <v>2010</v>
       </c>
       <c r="B13" s="43">
@@ -4424,7 +4402,7 @@
       <c r="L13" s="66"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="77">
+      <c r="A14" s="69">
         <v>2011</v>
       </c>
       <c r="B14" s="43">
@@ -4432,7 +4410,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="77">
+      <c r="A15" s="69">
         <v>2012</v>
       </c>
       <c r="B15" s="43">
@@ -4440,7 +4418,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="77">
+      <c r="A16" s="69">
         <v>2013</v>
       </c>
       <c r="B16" s="43">
@@ -4448,6 +4426,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="69"/>
       <c r="B17" s="43"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4556,10 +4535,10 @@
         <v>77</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="69" t="s">
+      <c r="H2" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="74"/>
+      <c r="I2" s="75"/>
       <c r="J2" s="4"/>
       <c r="K2" s="53" t="s">
         <v>84</v>
@@ -4590,10 +4569,10 @@
         <v>27852</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="75" t="s">
+      <c r="H3" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="76"/>
+      <c r="I3" s="77"/>
       <c r="J3" s="44"/>
       <c r="K3" s="56" t="s">
         <v>79</v>
@@ -11770,8 +11749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F423"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11813,8 +11792,14 @@
         <f>MID(F2,FIND("Plus",F2,1),LEN("plus"))</f>
         <v>Plus</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="D2" s="65" t="str">
+        <f>MID(F2,FIND("N",F2,1),1)</f>
+        <v>N</v>
+      </c>
+      <c r="E2" s="65">
+        <f>VLOOKUP(B2,'Warranty Sales'!$G$4:$I$17,IF('Data Parsing'!C2="Plus",2,3),FALSE)</f>
+        <v>200</v>
+      </c>
       <c r="F2" t="s">
         <v>88</v>
       </c>
@@ -11826,7 +11811,10 @@
         <v>17</v>
       </c>
       <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
+      <c r="D3" s="65">
+        <f>FIND("N",F2,1)</f>
+        <v>92</v>
+      </c>
       <c r="E3" s="65"/>
       <c r="F3" t="s">
         <v>89</v>
@@ -16067,11 +16055,11 @@
       <c r="B1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="72"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
@@ -16082,10 +16070,10 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="72" t="s">
+      <c r="H2" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="73"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="24"/>
@@ -22370,7 +22358,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>